<commit_message>
Sprint 1 - Fase Roja terminada
</commit_message>
<xml_diff>
--- a/docs/CasosPrueba - Estadística/CP - DesvSinSigno.xlsx
+++ b/docs/CasosPrueba - Estadística/CP - DesvSinSigno.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2cc5a38752f2b5bf/Ingeniería/Cuarto/Primer Cuatrimestre/Validación y Pruebas/Prácticas/Práctica 2/TDD-ACB-JGA/docs/CasosPrueba - Estadística/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adri_\source\repos\TDD-ACB-JGA\docs\CasosPrueba - Estadística\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="83" documentId="13_ncr:1_{D3CE32E0-4ADA-441D-8539-F74141AE4C58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9B15850D-2006-4B54-B6F5-D826325E07EC}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65281D94-76E0-46D9-8D1D-40308C439718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{12BA3133-949C-4B91-9275-35525239132A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{12BA3133-949C-4B91-9275-35525239132A}"/>
   </bookViews>
   <sheets>
     <sheet name="CP-001" sheetId="11" r:id="rId1"/>
@@ -185,12 +185,6 @@
     <t>Existe el método de calcularMedia</t>
   </si>
   <si>
-    <t>El método llama a calcularMediana</t>
-  </si>
-  <si>
-    <t>El método calcula la diferencia entre el valor devuelto y cada uno de los valores</t>
-  </si>
-  <si>
     <t>El método calcula el valor absoluto de cada uno de los elementos del vector</t>
   </si>
   <si>
@@ -207,6 +201,12 @@
   </si>
   <si>
     <t>RF-015</t>
+  </si>
+  <si>
+    <t>Se calcula la mediana del conjunto</t>
+  </si>
+  <si>
+    <t>El método calcula la diferencia entre el valor de la madiana y cada uno de los valores</t>
   </si>
 </sst>
 </file>
@@ -334,21 +334,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -361,14 +346,29 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -832,10 +832,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="17"/>
       <c r="D2" s="4" t="s">
         <v>28</v>
       </c>
@@ -847,10 +847,10 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="9"/>
+      <c r="C3" s="17"/>
       <c r="D3" s="4" t="s">
         <v>27</v>
       </c>
@@ -860,10 +860,10 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="17"/>
       <c r="D4" s="4" t="s">
         <v>26</v>
       </c>
@@ -871,89 +871,89 @@
         <v>16</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>1</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="17"/>
+      <c r="D13" s="12"/>
       <c r="E13" s="2" t="s">
         <v>8</v>
       </c>
@@ -965,10 +965,10 @@
       <c r="B14" s="6">
         <v>1</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="12"/>
+      <c r="D14" s="14"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
     </row>
@@ -976,10 +976,10 @@
       <c r="B15" s="6">
         <v>2</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="12"/>
+      <c r="D15" s="14"/>
       <c r="E15" s="7" t="s">
         <v>21</v>
       </c>
@@ -988,68 +988,68 @@
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="6">
         <v>1</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="14" t="s">
+      <c r="C20" s="11"/>
+      <c r="D20" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="15"/>
+      <c r="C22" s="10"/>
       <c r="D22" s="4" t="s">
         <v>19</v>
       </c>
@@ -1060,6 +1060,15 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B6:F8"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B9:F9"/>
     <mergeCell ref="D20:F21"/>
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B20:C21"/>
@@ -1070,15 +1079,6 @@
     <mergeCell ref="B16:F16"/>
     <mergeCell ref="C17:F17"/>
     <mergeCell ref="C18:F18"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B6:F8"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B9:F9"/>
   </mergeCells>
   <conditionalFormatting sqref="D22">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">
@@ -1113,10 +1113,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="17"/>
       <c r="D2" s="4" t="s">
         <v>28</v>
       </c>
@@ -1128,10 +1128,10 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="9"/>
+      <c r="C3" s="17"/>
       <c r="D3" s="4" t="s">
         <v>27</v>
       </c>
@@ -1141,10 +1141,10 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="17"/>
       <c r="D4" s="4" t="s">
         <v>26</v>
       </c>
@@ -1152,89 +1152,89 @@
         <v>16</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>1</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="17"/>
+      <c r="D13" s="12"/>
       <c r="E13" s="2" t="s">
         <v>8</v>
       </c>
@@ -1246,10 +1246,10 @@
       <c r="B14" s="6">
         <v>1</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="12"/>
+      <c r="D14" s="14"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
     </row>
@@ -1257,10 +1257,10 @@
       <c r="B15" s="6">
         <v>2</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="12"/>
+      <c r="D15" s="14"/>
       <c r="E15" s="7" t="s">
         <v>21</v>
       </c>
@@ -1269,68 +1269,68 @@
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="6">
         <v>1</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="14" t="s">
+      <c r="C20" s="11"/>
+      <c r="D20" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="15"/>
+      <c r="C22" s="10"/>
       <c r="D22" s="4" t="s">
         <v>19</v>
       </c>
@@ -1341,6 +1341,15 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F8"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="B22:C22"/>
@@ -1351,15 +1360,6 @@
     <mergeCell ref="B20:C21"/>
     <mergeCell ref="D20:F21"/>
     <mergeCell ref="C15:D15"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F8"/>
   </mergeCells>
   <conditionalFormatting sqref="D22">
     <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
@@ -1380,7 +1380,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C23DF389-A6B8-4FDE-A58B-49A12DA71E0E}">
   <dimension ref="B2:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -1394,10 +1394,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="17"/>
       <c r="D2" s="4" t="s">
         <v>28</v>
       </c>
@@ -1409,10 +1409,10 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="9"/>
+      <c r="C3" s="17"/>
       <c r="D3" s="4" t="s">
         <v>27</v>
       </c>
@@ -1422,10 +1422,10 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="17"/>
       <c r="D4" s="4" t="s">
         <v>26</v>
       </c>
@@ -1433,89 +1433,89 @@
         <v>16</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>1</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="10"/>
-      <c r="D12" s="10"/>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="15"/>
+      <c r="F12" s="15"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="17" t="s">
+      <c r="C13" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="17"/>
+      <c r="D13" s="12"/>
       <c r="E13" s="2" t="s">
         <v>8</v>
       </c>
@@ -1527,10 +1527,10 @@
       <c r="B14" s="6">
         <v>1</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D14" s="12"/>
+      <c r="D14" s="14"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
     </row>
@@ -1538,10 +1538,10 @@
       <c r="B15" s="6">
         <v>2</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="12"/>
+      <c r="D15" s="14"/>
       <c r="E15" s="7" t="s">
         <v>34</v>
       </c>
@@ -1550,68 +1550,68 @@
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="18" t="s">
+      <c r="B16" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="18"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
+      <c r="C16" s="16"/>
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="C17" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="17"/>
+      <c r="F17" s="17"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" s="6">
         <v>1</v>
       </c>
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
+      <c r="D18" s="19"/>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C20" s="16"/>
-      <c r="D20" s="14" t="s">
+      <c r="C20" s="11"/>
+      <c r="D20" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="E20" s="14"/>
-      <c r="F20" s="14"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="16"/>
-      <c r="C21" s="16"/>
-      <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="15"/>
+      <c r="C22" s="10"/>
       <c r="D22" s="4" t="s">
         <v>19</v>
       </c>
@@ -1622,6 +1622,15 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F8"/>
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="B22:C22"/>
@@ -1632,15 +1641,6 @@
     <mergeCell ref="B20:C21"/>
     <mergeCell ref="D20:F21"/>
     <mergeCell ref="C15:D15"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F8"/>
   </mergeCells>
   <conditionalFormatting sqref="D22">
     <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
@@ -1661,24 +1661,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1E4AD14-2046-48B4-AF6A-EE875681B014}">
   <dimension ref="B2:F28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="8" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" customWidth="1"/>
-    <col min="4" max="4" width="58.42578125" customWidth="1"/>
+    <col min="4" max="4" width="61.28515625" customWidth="1"/>
     <col min="5" max="5" width="37" customWidth="1"/>
     <col min="6" max="6" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="17"/>
       <c r="D2" s="4" t="s">
         <v>28</v>
       </c>
@@ -1690,10 +1690,10 @@
       </c>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="9"/>
+      <c r="C3" s="17"/>
       <c r="D3" s="4" t="s">
         <v>27</v>
       </c>
@@ -1703,10 +1703,10 @@
       <c r="F3" s="5"/>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="17"/>
       <c r="D4" s="4" t="s">
         <v>26</v>
       </c>
@@ -1714,111 +1714,111 @@
         <v>16</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="13"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="13"/>
-      <c r="F8" s="13"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="17"/>
+      <c r="F10" s="17"/>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>1</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
+      <c r="D11" s="14"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <v>2</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
+      <c r="D12" s="14"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
         <v>3</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="17" t="s">
+      <c r="C15" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="17"/>
+      <c r="D15" s="12"/>
       <c r="E15" s="2" t="s">
         <v>8</v>
       </c>
@@ -1830,10 +1830,10 @@
       <c r="B16" s="6">
         <v>1</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="12"/>
+      <c r="D16" s="14"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
     </row>
@@ -1841,10 +1841,10 @@
       <c r="B17" s="6">
         <v>2</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="C17" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="12"/>
+      <c r="D17" s="14"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
     </row>
@@ -1852,10 +1852,10 @@
       <c r="B18" s="6">
         <v>3</v>
       </c>
-      <c r="C18" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="D18" s="12"/>
+      <c r="C18" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="14"/>
       <c r="E18" s="7" t="s">
         <v>39</v>
       </c>
@@ -1868,7 +1868,7 @@
         <v>4</v>
       </c>
       <c r="C19" s="21" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="D19" s="22"/>
       <c r="E19" s="7"/>
@@ -1878,95 +1878,95 @@
       <c r="B20" s="6">
         <v>5</v>
       </c>
-      <c r="C20" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="D20" s="12"/>
+      <c r="C20" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="D20" s="14"/>
       <c r="E20" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B21" s="6">
         <v>6</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="D21" s="12"/>
+      <c r="C21" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="14"/>
       <c r="E21" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
+      <c r="C22" s="16"/>
+      <c r="D22" s="16"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="16"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="9" t="s">
+      <c r="C23" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B24" s="6">
         <v>1</v>
       </c>
-      <c r="C24" s="19" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
+      <c r="C24" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="19"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="19"/>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
+      <c r="C25" s="15"/>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+      <c r="F25" s="15"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="16" t="s">
+      <c r="B26" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C26" s="16"/>
-      <c r="D26" s="14" t="s">
+      <c r="C26" s="11"/>
+      <c r="D26" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="14"/>
-      <c r="F26" s="14"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="9"/>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B27" s="16"/>
-      <c r="C27" s="16"/>
-      <c r="D27" s="14"/>
-      <c r="E27" s="14"/>
-      <c r="F27" s="14"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C28" s="15"/>
+      <c r="C28" s="10"/>
       <c r="D28" s="4" t="s">
         <v>19</v>
       </c>
@@ -1977,6 +1977,18 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F8"/>
     <mergeCell ref="B28:C28"/>
     <mergeCell ref="C12:F12"/>
     <mergeCell ref="C18:D18"/>
@@ -1989,19 +2001,7 @@
     <mergeCell ref="B26:C27"/>
     <mergeCell ref="D26:F27"/>
     <mergeCell ref="C13:F13"/>
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F8"/>
     <mergeCell ref="C21:D21"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C10:F10"/>
   </mergeCells>
   <conditionalFormatting sqref="D28">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">

</xml_diff>